<commit_message>
updates with SHKs CD-64
</commit_message>
<xml_diff>
--- a/examples/lusid/holdings/_data/equity_holdings_20220301.xlsx
+++ b/examples/lusid/holdings/_data/equity_holdings_20220301.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25601"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10114"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\work\code\luminesce-examples\examples\lusid\holdings\_data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/oscarye/luminesce/luminesce-examples/examples/lusid/holdings/_data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B9CBA129-C78A-4FCE-AE6A-B72191FDFD91}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{55D85878-583D-CF47-B074-79CD8D9CEA74}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13896" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="5260" yWindow="2180" windowWidth="23260" windowHeight="13900" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="lusid_holdings" sheetId="1" r:id="rId1"/>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="259" uniqueCount="144">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="283" uniqueCount="148">
   <si>
     <t>InstrumentId</t>
   </si>
@@ -459,6 +459,18 @@
   </si>
   <si>
     <t>currency</t>
+  </si>
+  <si>
+    <t>strategy</t>
+  </si>
+  <si>
+    <t>Quantitative</t>
+  </si>
+  <si>
+    <t>Rebalance</t>
+  </si>
+  <si>
+    <t>Growth</t>
   </si>
 </sst>
 </file>
@@ -777,21 +789,21 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:D15"/>
+  <dimension ref="A1:E18"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E18" sqref="E18"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="13.77734375" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="25.21875" customWidth="1"/>
+    <col min="1" max="1" width="13.83203125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="25.1640625" customWidth="1"/>
     <col min="3" max="3" width="13.33203125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="4.6640625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="10.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>142</v>
       </c>
@@ -804,8 +816,11 @@
       <c r="D1" t="s">
         <v>143</v>
       </c>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="E1" t="s">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A2" s="1">
         <v>44621</v>
       </c>
@@ -818,8 +833,11 @@
       <c r="D2" t="s">
         <v>14</v>
       </c>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="E2" t="s">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A3" s="1">
         <v>44621</v>
       </c>
@@ -832,8 +850,11 @@
       <c r="D3" t="s">
         <v>14</v>
       </c>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="E3" t="s">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A4" s="1">
         <v>44621</v>
       </c>
@@ -846,8 +867,11 @@
       <c r="D4" t="s">
         <v>14</v>
       </c>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="E4" t="s">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A5" s="1">
         <v>44621</v>
       </c>
@@ -860,8 +884,11 @@
       <c r="D5" t="s">
         <v>14</v>
       </c>
-    </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="E5" t="s">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A6" s="1">
         <v>44621</v>
       </c>
@@ -874,8 +901,11 @@
       <c r="D6" t="s">
         <v>14</v>
       </c>
-    </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="E6" t="s">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A7" s="1">
         <v>44621</v>
       </c>
@@ -888,8 +918,11 @@
       <c r="D7" t="s">
         <v>14</v>
       </c>
-    </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="E7" t="s">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A8" s="1">
         <v>44621</v>
       </c>
@@ -902,8 +935,11 @@
       <c r="D8" t="s">
         <v>14</v>
       </c>
-    </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="E8" t="s">
+        <v>147</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A9" s="1">
         <v>44621</v>
       </c>
@@ -916,8 +952,11 @@
       <c r="D9" t="s">
         <v>14</v>
       </c>
-    </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="E9" t="s">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A10" s="1">
         <v>44621</v>
       </c>
@@ -930,8 +969,11 @@
       <c r="D10" t="s">
         <v>14</v>
       </c>
-    </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="E10" t="s">
+        <v>147</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A11" s="1">
         <v>44621</v>
       </c>
@@ -944,8 +986,11 @@
       <c r="D11" t="s">
         <v>14</v>
       </c>
-    </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="E11" t="s">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A12" s="1">
         <v>44621</v>
       </c>
@@ -958,8 +1003,11 @@
       <c r="D12" t="s">
         <v>14</v>
       </c>
-    </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="E12" t="s">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A13" s="1">
         <v>44621</v>
       </c>
@@ -972,8 +1020,11 @@
       <c r="D13" t="s">
         <v>14</v>
       </c>
-    </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="E13" t="s">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A14" s="1">
         <v>44621</v>
       </c>
@@ -986,8 +1037,11 @@
       <c r="D14" t="s">
         <v>14</v>
       </c>
-    </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="E14" t="s">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A15" s="1">
         <v>44621</v>
       </c>
@@ -999,6 +1053,60 @@
       </c>
       <c r="D15" t="s">
         <v>14</v>
+      </c>
+      <c r="E15" t="s">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A16" s="1">
+        <v>44621</v>
+      </c>
+      <c r="B16" t="s">
+        <v>83</v>
+      </c>
+      <c r="C16">
+        <v>1450</v>
+      </c>
+      <c r="D16" t="s">
+        <v>14</v>
+      </c>
+      <c r="E16" t="s">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A17" s="1">
+        <v>44621</v>
+      </c>
+      <c r="B17" t="s">
+        <v>76</v>
+      </c>
+      <c r="C17">
+        <v>790</v>
+      </c>
+      <c r="D17" t="s">
+        <v>14</v>
+      </c>
+      <c r="E17" t="s">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A18" s="1">
+        <v>44621</v>
+      </c>
+      <c r="B18" t="s">
+        <v>87</v>
+      </c>
+      <c r="C18">
+        <v>2300</v>
+      </c>
+      <c r="D18" t="s">
+        <v>14</v>
+      </c>
+      <c r="E18" t="s">
+        <v>147</v>
       </c>
     </row>
   </sheetData>
@@ -1010,21 +1118,21 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8A985CBD-E008-413F-8266-93F44EF3CE02}">
   <dimension ref="A1:G30"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B15" sqref="B15"/>
+    <sheetView topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="J13" sqref="J13:J14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="8.5546875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="26.109375" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="13.5546875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="8.5" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="26.1640625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="13.5" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="10.33203125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="20.109375" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="20.1640625" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="27.6640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>2</v>
       </c>
@@ -1047,7 +1155,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>9</v>
       </c>
@@ -1070,7 +1178,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>15</v>
       </c>
@@ -1093,7 +1201,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>22</v>
       </c>
@@ -1116,7 +1224,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>27</v>
       </c>
@@ -1139,7 +1247,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>32</v>
       </c>
@@ -1162,7 +1270,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>36</v>
       </c>
@@ -1185,7 +1293,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>40</v>
       </c>
@@ -1208,7 +1316,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>44</v>
       </c>
@@ -1231,7 +1339,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
         <v>48</v>
       </c>
@@ -1254,7 +1362,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
         <v>53</v>
       </c>
@@ -1277,7 +1385,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
         <v>59</v>
       </c>
@@ -1300,7 +1408,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
         <v>64</v>
       </c>
@@ -1323,7 +1431,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
         <v>68</v>
       </c>
@@ -1346,7 +1454,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
         <v>74</v>
       </c>
@@ -1369,7 +1477,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
         <v>78</v>
       </c>
@@ -1392,7 +1500,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="17" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
         <v>81</v>
       </c>
@@ -1415,7 +1523,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="18" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
         <v>85</v>
       </c>
@@ -1438,7 +1546,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="19" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
         <v>89</v>
       </c>
@@ -1461,7 +1569,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="20" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
         <v>93</v>
       </c>
@@ -1484,7 +1592,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="21" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
         <v>99</v>
       </c>
@@ -1507,7 +1615,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="22" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
         <v>104</v>
       </c>
@@ -1530,7 +1638,7 @@
         <v>107</v>
       </c>
     </row>
-    <row r="23" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
         <v>108</v>
       </c>
@@ -1553,7 +1661,7 @@
         <v>107</v>
       </c>
     </row>
-    <row r="24" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
         <v>113</v>
       </c>
@@ -1576,7 +1684,7 @@
         <v>107</v>
       </c>
     </row>
-    <row r="25" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
         <v>117</v>
       </c>
@@ -1599,7 +1707,7 @@
         <v>107</v>
       </c>
     </row>
-    <row r="26" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
         <v>122</v>
       </c>
@@ -1622,7 +1730,7 @@
         <v>126</v>
       </c>
     </row>
-    <row r="27" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
         <v>127</v>
       </c>
@@ -1645,7 +1753,7 @@
         <v>126</v>
       </c>
     </row>
-    <row r="28" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A28" t="s">
         <v>130</v>
       </c>
@@ -1668,7 +1776,7 @@
         <v>126</v>
       </c>
     </row>
-    <row r="29" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A29" t="s">
         <v>134</v>
       </c>
@@ -1691,7 +1799,7 @@
         <v>138</v>
       </c>
     </row>
-    <row r="30" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A30" t="s">
         <v>139</v>
       </c>
@@ -1724,17 +1832,17 @@
   <dimension ref="A1:D15"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E4" sqref="E4"/>
+      <selection activeCell="B13" sqref="B13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="13.77734375" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="17.77734375" customWidth="1"/>
+    <col min="1" max="1" width="13.83203125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="17.83203125" customWidth="1"/>
     <col min="3" max="3" width="13.33203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>142</v>
       </c>
@@ -1748,7 +1856,7 @@
         <v>143</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A2" s="1">
         <v>44621</v>
       </c>
@@ -1762,7 +1870,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A3" s="1">
         <v>44621</v>
       </c>
@@ -1776,7 +1884,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A4" s="1">
         <v>44621</v>
       </c>
@@ -1790,7 +1898,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A5" s="1">
         <v>44621</v>
       </c>
@@ -1804,7 +1912,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A6" s="1">
         <v>44621</v>
       </c>
@@ -1818,7 +1926,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A7" s="1">
         <v>44621</v>
       </c>
@@ -1832,7 +1940,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A8" s="1">
         <v>44621</v>
       </c>
@@ -1846,7 +1954,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A9" s="1">
         <v>44621</v>
       </c>
@@ -1860,7 +1968,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A10" s="1">
         <v>44621</v>
       </c>
@@ -1874,7 +1982,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A11" s="1">
         <v>44621</v>
       </c>
@@ -1888,7 +1996,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A12" s="1">
         <v>44621</v>
       </c>
@@ -1902,7 +2010,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A13" s="1">
         <v>44621</v>
       </c>
@@ -1916,7 +2024,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A14" s="1">
         <v>44621</v>
       </c>
@@ -1930,7 +2038,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A15" s="1">
         <v>44621</v>
       </c>

</xml_diff>

<commit_message>
updates with SHKs CD-64 (#148)
* updates with SHKs CD-64

* updates per comments

* Delete examples/lusid/holdings/.DS_Store

* Delete examples/.DS_Store

* Delete examples/lusid/.DS_Store

* Delete .DS_Store
</commit_message>
<xml_diff>
--- a/examples/lusid/holdings/_data/equity_holdings_20220301.xlsx
+++ b/examples/lusid/holdings/_data/equity_holdings_20220301.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25601"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10114"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\work\code\luminesce-examples\examples\lusid\holdings\_data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/oscarye/luminesce/luminesce-examples/examples/lusid/holdings/_data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B9CBA129-C78A-4FCE-AE6A-B72191FDFD91}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{55D85878-583D-CF47-B074-79CD8D9CEA74}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13896" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="5260" yWindow="2180" windowWidth="23260" windowHeight="13900" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="lusid_holdings" sheetId="1" r:id="rId1"/>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="259" uniqueCount="144">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="283" uniqueCount="148">
   <si>
     <t>InstrumentId</t>
   </si>
@@ -459,6 +459,18 @@
   </si>
   <si>
     <t>currency</t>
+  </si>
+  <si>
+    <t>strategy</t>
+  </si>
+  <si>
+    <t>Quantitative</t>
+  </si>
+  <si>
+    <t>Rebalance</t>
+  </si>
+  <si>
+    <t>Growth</t>
   </si>
 </sst>
 </file>
@@ -777,21 +789,21 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:D15"/>
+  <dimension ref="A1:E18"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E18" sqref="E18"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="13.77734375" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="25.21875" customWidth="1"/>
+    <col min="1" max="1" width="13.83203125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="25.1640625" customWidth="1"/>
     <col min="3" max="3" width="13.33203125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="4.6640625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="10.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>142</v>
       </c>
@@ -804,8 +816,11 @@
       <c r="D1" t="s">
         <v>143</v>
       </c>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="E1" t="s">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A2" s="1">
         <v>44621</v>
       </c>
@@ -818,8 +833,11 @@
       <c r="D2" t="s">
         <v>14</v>
       </c>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="E2" t="s">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A3" s="1">
         <v>44621</v>
       </c>
@@ -832,8 +850,11 @@
       <c r="D3" t="s">
         <v>14</v>
       </c>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="E3" t="s">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A4" s="1">
         <v>44621</v>
       </c>
@@ -846,8 +867,11 @@
       <c r="D4" t="s">
         <v>14</v>
       </c>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="E4" t="s">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A5" s="1">
         <v>44621</v>
       </c>
@@ -860,8 +884,11 @@
       <c r="D5" t="s">
         <v>14</v>
       </c>
-    </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="E5" t="s">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A6" s="1">
         <v>44621</v>
       </c>
@@ -874,8 +901,11 @@
       <c r="D6" t="s">
         <v>14</v>
       </c>
-    </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="E6" t="s">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A7" s="1">
         <v>44621</v>
       </c>
@@ -888,8 +918,11 @@
       <c r="D7" t="s">
         <v>14</v>
       </c>
-    </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="E7" t="s">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A8" s="1">
         <v>44621</v>
       </c>
@@ -902,8 +935,11 @@
       <c r="D8" t="s">
         <v>14</v>
       </c>
-    </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="E8" t="s">
+        <v>147</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A9" s="1">
         <v>44621</v>
       </c>
@@ -916,8 +952,11 @@
       <c r="D9" t="s">
         <v>14</v>
       </c>
-    </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="E9" t="s">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A10" s="1">
         <v>44621</v>
       </c>
@@ -930,8 +969,11 @@
       <c r="D10" t="s">
         <v>14</v>
       </c>
-    </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="E10" t="s">
+        <v>147</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A11" s="1">
         <v>44621</v>
       </c>
@@ -944,8 +986,11 @@
       <c r="D11" t="s">
         <v>14</v>
       </c>
-    </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="E11" t="s">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A12" s="1">
         <v>44621</v>
       </c>
@@ -958,8 +1003,11 @@
       <c r="D12" t="s">
         <v>14</v>
       </c>
-    </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="E12" t="s">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A13" s="1">
         <v>44621</v>
       </c>
@@ -972,8 +1020,11 @@
       <c r="D13" t="s">
         <v>14</v>
       </c>
-    </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="E13" t="s">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A14" s="1">
         <v>44621</v>
       </c>
@@ -986,8 +1037,11 @@
       <c r="D14" t="s">
         <v>14</v>
       </c>
-    </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="E14" t="s">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A15" s="1">
         <v>44621</v>
       </c>
@@ -999,6 +1053,60 @@
       </c>
       <c r="D15" t="s">
         <v>14</v>
+      </c>
+      <c r="E15" t="s">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A16" s="1">
+        <v>44621</v>
+      </c>
+      <c r="B16" t="s">
+        <v>83</v>
+      </c>
+      <c r="C16">
+        <v>1450</v>
+      </c>
+      <c r="D16" t="s">
+        <v>14</v>
+      </c>
+      <c r="E16" t="s">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A17" s="1">
+        <v>44621</v>
+      </c>
+      <c r="B17" t="s">
+        <v>76</v>
+      </c>
+      <c r="C17">
+        <v>790</v>
+      </c>
+      <c r="D17" t="s">
+        <v>14</v>
+      </c>
+      <c r="E17" t="s">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A18" s="1">
+        <v>44621</v>
+      </c>
+      <c r="B18" t="s">
+        <v>87</v>
+      </c>
+      <c r="C18">
+        <v>2300</v>
+      </c>
+      <c r="D18" t="s">
+        <v>14</v>
+      </c>
+      <c r="E18" t="s">
+        <v>147</v>
       </c>
     </row>
   </sheetData>
@@ -1010,21 +1118,21 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8A985CBD-E008-413F-8266-93F44EF3CE02}">
   <dimension ref="A1:G30"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B15" sqref="B15"/>
+    <sheetView topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="J13" sqref="J13:J14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="8.5546875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="26.109375" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="13.5546875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="8.5" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="26.1640625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="13.5" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="10.33203125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="20.109375" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="20.1640625" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="27.6640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>2</v>
       </c>
@@ -1047,7 +1155,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>9</v>
       </c>
@@ -1070,7 +1178,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>15</v>
       </c>
@@ -1093,7 +1201,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>22</v>
       </c>
@@ -1116,7 +1224,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>27</v>
       </c>
@@ -1139,7 +1247,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>32</v>
       </c>
@@ -1162,7 +1270,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>36</v>
       </c>
@@ -1185,7 +1293,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>40</v>
       </c>
@@ -1208,7 +1316,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>44</v>
       </c>
@@ -1231,7 +1339,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
         <v>48</v>
       </c>
@@ -1254,7 +1362,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
         <v>53</v>
       </c>
@@ -1277,7 +1385,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
         <v>59</v>
       </c>
@@ -1300,7 +1408,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
         <v>64</v>
       </c>
@@ -1323,7 +1431,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
         <v>68</v>
       </c>
@@ -1346,7 +1454,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
         <v>74</v>
       </c>
@@ -1369,7 +1477,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
         <v>78</v>
       </c>
@@ -1392,7 +1500,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="17" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
         <v>81</v>
       </c>
@@ -1415,7 +1523,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="18" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
         <v>85</v>
       </c>
@@ -1438,7 +1546,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="19" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
         <v>89</v>
       </c>
@@ -1461,7 +1569,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="20" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
         <v>93</v>
       </c>
@@ -1484,7 +1592,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="21" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
         <v>99</v>
       </c>
@@ -1507,7 +1615,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="22" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
         <v>104</v>
       </c>
@@ -1530,7 +1638,7 @@
         <v>107</v>
       </c>
     </row>
-    <row r="23" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
         <v>108</v>
       </c>
@@ -1553,7 +1661,7 @@
         <v>107</v>
       </c>
     </row>
-    <row r="24" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
         <v>113</v>
       </c>
@@ -1576,7 +1684,7 @@
         <v>107</v>
       </c>
     </row>
-    <row r="25" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
         <v>117</v>
       </c>
@@ -1599,7 +1707,7 @@
         <v>107</v>
       </c>
     </row>
-    <row r="26" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
         <v>122</v>
       </c>
@@ -1622,7 +1730,7 @@
         <v>126</v>
       </c>
     </row>
-    <row r="27" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
         <v>127</v>
       </c>
@@ -1645,7 +1753,7 @@
         <v>126</v>
       </c>
     </row>
-    <row r="28" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A28" t="s">
         <v>130</v>
       </c>
@@ -1668,7 +1776,7 @@
         <v>126</v>
       </c>
     </row>
-    <row r="29" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A29" t="s">
         <v>134</v>
       </c>
@@ -1691,7 +1799,7 @@
         <v>138</v>
       </c>
     </row>
-    <row r="30" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A30" t="s">
         <v>139</v>
       </c>
@@ -1724,17 +1832,17 @@
   <dimension ref="A1:D15"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E4" sqref="E4"/>
+      <selection activeCell="B13" sqref="B13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="13.77734375" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="17.77734375" customWidth="1"/>
+    <col min="1" max="1" width="13.83203125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="17.83203125" customWidth="1"/>
     <col min="3" max="3" width="13.33203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>142</v>
       </c>
@@ -1748,7 +1856,7 @@
         <v>143</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A2" s="1">
         <v>44621</v>
       </c>
@@ -1762,7 +1870,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A3" s="1">
         <v>44621</v>
       </c>
@@ -1776,7 +1884,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A4" s="1">
         <v>44621</v>
       </c>
@@ -1790,7 +1898,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A5" s="1">
         <v>44621</v>
       </c>
@@ -1804,7 +1912,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A6" s="1">
         <v>44621</v>
       </c>
@@ -1818,7 +1926,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A7" s="1">
         <v>44621</v>
       </c>
@@ -1832,7 +1940,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A8" s="1">
         <v>44621</v>
       </c>
@@ -1846,7 +1954,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A9" s="1">
         <v>44621</v>
       </c>
@@ -1860,7 +1968,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A10" s="1">
         <v>44621</v>
       </c>
@@ -1874,7 +1982,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A11" s="1">
         <v>44621</v>
       </c>
@@ -1888,7 +1996,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A12" s="1">
         <v>44621</v>
       </c>
@@ -1902,7 +2010,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A13" s="1">
         <v>44621</v>
       </c>
@@ -1916,7 +2024,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A14" s="1">
         <v>44621</v>
       </c>
@@ -1930,7 +2038,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A15" s="1">
         <v>44621</v>
       </c>

</xml_diff>